<commit_message>
Added planned points to punktesystem
</commit_message>
<xml_diff>
--- a/frontend/punktesystem.xlsx
+++ b/frontend/punktesystem.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Master\3_Semester\Online_Multimedia\Übung\grouptask02\frontend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steffi/Documents/LMU/Master/3_FS/OMM/grouptask02/frontend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{909EC18A-5C03-4D97-8240-EB33D9BFC45B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06530A82-C5FC-1240-9D63-364FB0B0F339}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{221AE7D0-B4E4-410E-BBC6-994CE88AAB86}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{221AE7D0-B4E4-410E-BBC6-994CE88AAB86}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="83">
   <si>
     <t>Feature list</t>
   </si>
@@ -280,13 +280,16 @@
   </si>
   <si>
     <t>Complex</t>
+  </si>
+  <si>
+    <t>Planned points</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,6 +338,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -356,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -371,13 +381,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,7 +404,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -689,29 +700,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75FC8529-C13A-4402-B272-4F9116FF34D2}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="121.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="5"/>
-    <col min="3" max="3" width="18.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="113.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="121.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="5"/>
+    <col min="3" max="4" width="18.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="113.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -721,11 +733,14 @@
       <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -735,11 +750,14 @@
       <c r="C3" s="7">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -749,8 +767,11 @@
       <c r="C4" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -760,41 +781,51 @@
       <c r="C5" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="5">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="10">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -804,11 +835,14 @@
       <c r="C9" s="7">
         <v>1</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -818,8 +852,11 @@
       <c r="C10" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -829,8 +866,11 @@
       <c r="C11" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -840,8 +880,11 @@
       <c r="C12" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -851,11 +894,14 @@
       <c r="C13" s="7">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="7">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -865,33 +911,42 @@
       <c r="C14" s="7">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="7">
         <v>3</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="7">
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B16" s="7">
         <v>4</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="7">
+        <v>4</v>
+      </c>
+      <c r="E16" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -899,18 +954,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="7">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="7">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -918,7 +976,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
@@ -926,11 +984,14 @@
         <v>1</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -938,8 +999,9 @@
         <v>1</v>
       </c>
       <c r="C21" s="7"/>
-    </row>
-    <row r="22" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -947,8 +1009,9 @@
         <v>2</v>
       </c>
       <c r="C22" s="7"/>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>25</v>
       </c>
@@ -956,11 +1019,14 @@
         <v>1</v>
       </c>
       <c r="C23" s="7"/>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="7">
+        <v>1</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="24" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -968,11 +1034,14 @@
         <v>1</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="9" t="s">
+      <c r="D24" s="7">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -980,8 +1049,9 @@
         <v>1</v>
       </c>
       <c r="C25" s="7"/>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>28</v>
       </c>
@@ -991,11 +1061,14 @@
       <c r="C26" s="7">
         <v>1</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D26" s="7">
+        <v>1</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
@@ -1005,8 +1078,11 @@
       <c r="C27" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -1014,8 +1090,9 @@
         <v>3</v>
       </c>
       <c r="C28" s="7"/>
-    </row>
-    <row r="29" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>31</v>
       </c>
@@ -1023,11 +1100,14 @@
         <v>1</v>
       </c>
       <c r="C29" s="7"/>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
@@ -1035,8 +1115,9 @@
         <v>2</v>
       </c>
       <c r="C30" s="7"/>
-    </row>
-    <row r="31" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
@@ -1046,8 +1127,11 @@
       <c r="C31" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>34</v>
       </c>
@@ -1055,8 +1139,9 @@
         <v>1</v>
       </c>
       <c r="C32" s="7"/>
-    </row>
-    <row r="33" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
@@ -1064,8 +1149,9 @@
         <v>3</v>
       </c>
       <c r="C33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>36</v>
       </c>
@@ -1073,8 +1159,11 @@
         <v>1</v>
       </c>
       <c r="C34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
@@ -1082,8 +1171,9 @@
         <v>2</v>
       </c>
       <c r="C35" s="7"/>
-    </row>
-    <row r="36" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
@@ -1091,11 +1181,14 @@
         <v>1</v>
       </c>
       <c r="C36" s="7"/>
-      <c r="D36" s="9" t="s">
+      <c r="D36" s="7">
+        <v>1</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="1" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -1103,8 +1196,11 @@
         <v>2</v>
       </c>
       <c r="C37" s="7"/>
-    </row>
-    <row r="38" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>40</v>
       </c>
@@ -1112,8 +1208,11 @@
         <v>2</v>
       </c>
       <c r="C38" s="7"/>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -1121,8 +1220,11 @@
         <v>2</v>
       </c>
       <c r="C39" s="7"/>
-    </row>
-    <row r="40" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -1130,8 +1232,9 @@
         <v>2</v>
       </c>
       <c r="C40" s="7"/>
-    </row>
-    <row r="41" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="7"/>
+    </row>
+    <row r="41" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -1139,8 +1242,9 @@
         <v>2</v>
       </c>
       <c r="C41" s="7"/>
-    </row>
-    <row r="42" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="7"/>
+    </row>
+    <row r="42" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -1148,8 +1252,11 @@
         <v>2</v>
       </c>
       <c r="C42" s="7"/>
-    </row>
-    <row r="43" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>45</v>
       </c>
@@ -1157,8 +1264,9 @@
         <v>2</v>
       </c>
       <c r="C43" s="7"/>
-    </row>
-    <row r="44" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="7"/>
+    </row>
+    <row r="44" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>46</v>
       </c>
@@ -1166,8 +1274,9 @@
         <v>3</v>
       </c>
       <c r="C44" s="7"/>
-    </row>
-    <row r="45" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="7"/>
+    </row>
+    <row r="45" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>47</v>
       </c>
@@ -1175,8 +1284,9 @@
         <v>2</v>
       </c>
       <c r="C45" s="7"/>
-    </row>
-    <row r="46" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="7"/>
+    </row>
+    <row r="46" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>48</v>
       </c>
@@ -1184,8 +1294,9 @@
         <v>2</v>
       </c>
       <c r="C46" s="7"/>
-    </row>
-    <row r="47" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="7"/>
+    </row>
+    <row r="47" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>49</v>
       </c>
@@ -1193,8 +1304,9 @@
         <v>5</v>
       </c>
       <c r="C47" s="7"/>
-    </row>
-    <row r="48" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="7"/>
+    </row>
+    <row r="48" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>50</v>
       </c>
@@ -1202,11 +1314,12 @@
         <v>3</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="1" t="s">
+      <c r="D48" s="7"/>
+      <c r="E48" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>51</v>
       </c>
@@ -1214,8 +1327,9 @@
         <v>1</v>
       </c>
       <c r="C49" s="7"/>
-    </row>
-    <row r="50" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="7"/>
+    </row>
+    <row r="50" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
         <v>52</v>
       </c>
@@ -1223,8 +1337,9 @@
         <v>2</v>
       </c>
       <c r="C50" s="7"/>
-    </row>
-    <row r="51" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="7"/>
+    </row>
+    <row r="51" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>53</v>
       </c>
@@ -1232,8 +1347,9 @@
         <v>2</v>
       </c>
       <c r="C51" s="7"/>
-    </row>
-    <row r="52" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D51" s="7"/>
+    </row>
+    <row r="52" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>54</v>
       </c>
@@ -1241,8 +1357,9 @@
         <v>1</v>
       </c>
       <c r="C52" s="7"/>
-    </row>
-    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D52" s="7"/>
+    </row>
+    <row r="53" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
@@ -1250,8 +1367,9 @@
         <v>3</v>
       </c>
       <c r="C53" s="7"/>
-    </row>
-    <row r="54" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>56</v>
       </c>
@@ -1259,8 +1377,9 @@
         <v>5</v>
       </c>
       <c r="C54" s="7"/>
-    </row>
-    <row r="55" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="7"/>
+    </row>
+    <row r="55" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>57</v>
       </c>
@@ -1268,11 +1387,14 @@
         <v>5</v>
       </c>
       <c r="C55" s="7"/>
-      <c r="D55" s="1" t="s">
+      <c r="D55" s="7">
+        <v>5</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
@@ -1280,11 +1402,12 @@
         <v>10</v>
       </c>
       <c r="C56" s="7"/>
-      <c r="D56" s="1" t="s">
+      <c r="D56" s="7"/>
+      <c r="E56" s="1" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>59</v>
       </c>
@@ -1292,8 +1415,9 @@
         <v>4</v>
       </c>
       <c r="C57" s="7"/>
-    </row>
-    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="7"/>
+    </row>
+    <row r="58" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>60</v>
       </c>
@@ -1301,8 +1425,9 @@
         <v>5</v>
       </c>
       <c r="C58" s="7"/>
-    </row>
-    <row r="59" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D58" s="7"/>
+    </row>
+    <row r="59" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>61</v>
       </c>
@@ -1310,8 +1435,9 @@
         <v>3</v>
       </c>
       <c r="C59" s="7"/>
-    </row>
-    <row r="60" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D59" s="7"/>
+    </row>
+    <row r="60" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>62</v>
       </c>
@@ -1319,8 +1445,9 @@
         <v>3</v>
       </c>
       <c r="C60" s="7"/>
-    </row>
-    <row r="61" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D60" s="7"/>
+    </row>
+    <row r="61" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>63</v>
       </c>
@@ -1330,8 +1457,11 @@
       <c r="C61" s="7">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D61" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>64</v>
       </c>
@@ -1339,8 +1469,11 @@
         <v>2</v>
       </c>
       <c r="C62" s="7"/>
-    </row>
-    <row r="63" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D62" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>65</v>
       </c>
@@ -1348,8 +1481,11 @@
         <v>2</v>
       </c>
       <c r="C63" s="7"/>
-    </row>
-    <row r="64" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D63" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
@@ -1357,8 +1493,11 @@
         <v>2</v>
       </c>
       <c r="C64" s="7"/>
-    </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="5">
         <f>SUM(B3:B64)</f>
         <v>135</v>
@@ -1367,8 +1506,12 @@
         <f>SUM(C3:C64)</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="7">
+        <f>SUM(D3:D64)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="5" t="s">
         <v>11</v>
       </c>
@@ -1379,7 +1522,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>